<commit_message>
consegui refazer a rede de um modelo escolhido, apresentar seu mse_sup e 3d
</commit_message>
<xml_diff>
--- a/Peaks-dataset-article/redes-ensemble/Teste05/better_results.xlsx
+++ b/Peaks-dataset-article/redes-ensemble/Teste05/better_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -527,322 +527,322 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>model_22_9_7</t>
+          <t>model_22_9_0</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.9997735427952396</v>
+        <v>0.9998401530247623</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8534547500861769</v>
+        <v>0.8251524996196588</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9993299854719881</v>
+        <v>0.9986200337059677</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9992796260654657</v>
+        <v>0.9997296204734236</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9995126019313403</v>
+        <v>0.9994282459175685</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0003214231293374287</v>
+        <v>0.0002268795777567717</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2079997095551038</v>
+        <v>0.2481706457011295</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0005950044635148943</v>
+        <v>0.00107181206659941</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0007110608698974434</v>
+        <v>0.0003461839329454344</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0006530315747155433</v>
+        <v>0.0007090023618995093</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0546178350608918</v>
+        <v>0.01329431775750658</v>
       </c>
       <c r="N2" t="n">
-        <v>0.01792827736670282</v>
+        <v>0.01506252229066472</v>
       </c>
       <c r="O2" t="n">
-        <v>1.000013971652736</v>
+        <v>1.000006625781357</v>
       </c>
       <c r="P2" t="n">
-        <v>0.01869152125085377</v>
+        <v>0.01570376504829791</v>
       </c>
       <c r="Q2" t="n">
-        <v>842.0855042858293</v>
+        <v>1222.782182351417</v>
       </c>
       <c r="R2" t="n">
-        <v>1345.481219956396</v>
+        <v>1957.764304746942</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>model_22_9_8</t>
+          <t>model_22_9_1</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.9997733662200464</v>
+        <v>0.999840148582673</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8536790466810209</v>
+        <v>0.8251525175977871</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9992225433726208</v>
+        <v>0.9986199949681903</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9992393103296912</v>
+        <v>0.9997296141287978</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9994621438299516</v>
+        <v>0.9994282310207155</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0003216737521921262</v>
+        <v>0.0002268858826577248</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2076813530979058</v>
+        <v>0.2481706201837861</v>
       </c>
       <c r="J3" t="n">
-        <v>0.000690418109070703</v>
+        <v>0.001071842154013507</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0007508553998993933</v>
+        <v>0.0003461920563692762</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0007206369583348119</v>
+        <v>0.0007090208347085881</v>
       </c>
       <c r="M3" t="n">
-        <v>0.05085987027780254</v>
+        <v>0.01329491784952716</v>
       </c>
       <c r="N3" t="n">
-        <v>0.01793526560138227</v>
+        <v>0.01506273158021893</v>
       </c>
       <c r="O3" t="n">
-        <v>1.000013982546835</v>
+        <v>1.000006625965485</v>
       </c>
       <c r="P3" t="n">
-        <v>0.01869880698915117</v>
+        <v>0.01570398324774173</v>
       </c>
       <c r="Q3" t="n">
-        <v>842.0839454359914</v>
+        <v>1222.782126772916</v>
       </c>
       <c r="R3" t="n">
-        <v>1345.479661106558</v>
+        <v>1957.764249168441</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>model_22_9_9</t>
+          <t>model_22_9_2</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.9997708857164302</v>
+        <v>0.9998401445090002</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8538785985469226</v>
+        <v>0.8251525190435377</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9991187574968349</v>
+        <v>0.9986199573951215</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9992007414643671</v>
+        <v>0.9997296047398737</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9994135410683828</v>
+        <v>0.9994282174412299</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0003251944670022894</v>
+        <v>0.0002268916646449084</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2073981181914648</v>
+        <v>0.248170618131753</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0007825848558511373</v>
+        <v>0.001071871336804853</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0007889256431626703</v>
+        <v>0.0003462040776000099</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0007857564981189119</v>
+        <v>0.0007090376739191662</v>
       </c>
       <c r="M4" t="n">
-        <v>0.04747471697922476</v>
+        <v>0.01329303698821029</v>
       </c>
       <c r="N4" t="n">
-        <v>0.01803314911495742</v>
+        <v>0.01506292350922982</v>
       </c>
       <c r="O4" t="n">
-        <v>1.000014135585619</v>
+        <v>1.000006626134342</v>
       </c>
       <c r="P4" t="n">
-        <v>0.01880085760654601</v>
+        <v>0.01570418334756796</v>
       </c>
       <c r="Q4" t="n">
-        <v>842.0621743891469</v>
+        <v>1222.782075805325</v>
       </c>
       <c r="R4" t="n">
-        <v>1345.457890059714</v>
+        <v>1957.76419820085</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>model_22_9_6</t>
+          <t>model_22_9_3</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.9997705556121292</v>
+        <v>0.9998401431215934</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8532022215858097</v>
+        <v>0.8251525312322723</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9994397150571014</v>
+        <v>0.9986199390930662</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9993212768565715</v>
+        <v>0.9997296042513145</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9995643093028377</v>
+        <v>0.9994282134714005</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0003256630021391189</v>
+        <v>0.0002268936338674635</v>
       </c>
       <c r="I5" t="n">
-        <v>0.208358137104012</v>
+        <v>0.2481706008316136</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0004975594228592668</v>
+        <v>0.001071885551908407</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0006699485442902188</v>
+        <v>0.0003462047031330931</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0005837523789112587</v>
+        <v>0.0007090425966970685</v>
       </c>
       <c r="M5" t="n">
-        <v>0.05879080007762785</v>
+        <v>0.01329375605002713</v>
       </c>
       <c r="N5" t="n">
-        <v>0.01804613537960743</v>
+        <v>0.01506298887563366</v>
       </c>
       <c r="O5" t="n">
-        <v>1.000014155951951</v>
+        <v>1.000006626191851</v>
       </c>
       <c r="P5" t="n">
-        <v>0.01881439672336745</v>
+        <v>0.01570425149675495</v>
       </c>
       <c r="Q5" t="n">
-        <v>842.0592948940809</v>
+        <v>1222.782058447137</v>
       </c>
       <c r="R5" t="n">
-        <v>1345.455010564648</v>
+        <v>1957.764180842662</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>model_22_9_10</t>
+          <t>model_22_9_4</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.9997667641359308</v>
+        <v>0.9998401396198875</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8540562363254669</v>
+        <v>0.8251525477035119</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9990195780354975</v>
+        <v>0.9986199129522194</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9991641612583444</v>
+        <v>0.9997295997987813</v>
       </c>
       <c r="G6" t="n">
-        <v>0.999367198149245</v>
+        <v>0.9994282009452882</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0003310444522272507</v>
+        <v>0.0002268986040306357</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2071459871509503</v>
+        <v>0.2481705774530799</v>
       </c>
       <c r="J6" t="n">
-        <v>0.000870660889605</v>
+        <v>0.001071905855357254</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0008250329367065158</v>
+        <v>0.000346210403991845</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0008478482284877287</v>
+        <v>0.0007090581296745494</v>
       </c>
       <c r="M6" t="n">
-        <v>0.04443492416787045</v>
+        <v>0.0132938924193047</v>
       </c>
       <c r="N6" t="n">
-        <v>0.01819462701533754</v>
+        <v>0.01506315385404517</v>
       </c>
       <c r="O6" t="n">
-        <v>1.000014389873362</v>
+        <v>1.000006626337</v>
       </c>
       <c r="P6" t="n">
-        <v>0.01896920995545065</v>
+        <v>0.01570442349863898</v>
       </c>
       <c r="Q6" t="n">
-        <v>842.0265157896903</v>
+        <v>1222.782014637105</v>
       </c>
       <c r="R6" t="n">
-        <v>1345.422231460257</v>
+        <v>1957.76413703263</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -850,686 +850,1379 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9997633163694918</v>
+        <v>0.9998401374163525</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8529176445093882</v>
+        <v>0.8251525701206495</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9995497563938098</v>
+        <v>0.9986199059522779</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9993636885294639</v>
+        <v>0.9997295887752294</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9996163986850612</v>
+        <v>0.9994281930621389</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0003359380562052841</v>
+        <v>0.0002269017316287704</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2087620529544168</v>
+        <v>0.2481705456352072</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0003998375321012418</v>
+        <v>0.001071911292172465</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0006280851736503217</v>
+        <v>0.0003462245181393473</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0005139613528757817</v>
+        <v>0.0007090679051559061</v>
       </c>
       <c r="M7" t="n">
-        <v>0.06343471411977647</v>
+        <v>0.0132934884423456</v>
       </c>
       <c r="N7" t="n">
-        <v>0.01832861304641691</v>
+        <v>0.01506325766986578</v>
       </c>
       <c r="O7" t="n">
-        <v>1.000014602589029</v>
+        <v>1.000006626428338</v>
       </c>
       <c r="P7" t="n">
-        <v>0.01910890004926239</v>
+        <v>0.01570453173411401</v>
       </c>
       <c r="Q7" t="n">
-        <v>841.9971675430575</v>
+        <v>1222.78198706905</v>
       </c>
       <c r="R7" t="n">
-        <v>1345.392883213624</v>
+        <v>1957.764109464575</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>model_22_9_4</t>
+          <t>model_22_9_6</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.9997504365126391</v>
+        <v>0.9998401365512083</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8525964631431158</v>
+        <v>0.8251526053388949</v>
       </c>
       <c r="E8" t="n">
-        <v>0.999657503429227</v>
+        <v>0.9986198913815635</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9994060159908327</v>
+        <v>0.9997295925559928</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9996676979398783</v>
+        <v>0.999428190961085</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0003542191433509788</v>
+        <v>0.0002269029595752931</v>
       </c>
       <c r="I8" t="n">
-        <v>0.209217923280739</v>
+        <v>0.2481704956480202</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0003041530889683757</v>
+        <v>0.001071922609164532</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0005863049258393546</v>
+        <v>0.0003462196773899201</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0004452289648976248</v>
+        <v>0.000709070510563141</v>
       </c>
       <c r="M8" t="n">
-        <v>0.06859671046370525</v>
+        <v>0.01329178747791211</v>
       </c>
       <c r="N8" t="n">
-        <v>0.01882071049006862</v>
+        <v>0.01506329842947066</v>
       </c>
       <c r="O8" t="n">
-        <v>1.000015397233153</v>
+        <v>1.000006626464199</v>
       </c>
       <c r="P8" t="n">
-        <v>0.01962194709987249</v>
+        <v>0.01570457422893964</v>
       </c>
       <c r="Q8" t="n">
-        <v>841.8911895746965</v>
+        <v>1222.781976245482</v>
       </c>
       <c r="R8" t="n">
-        <v>1345.286905245263</v>
+        <v>1957.764098641007</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>model_22_9_3</t>
+          <t>model_22_9_7</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.9997301696369398</v>
+        <v>0.9998401338544861</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8522334759911255</v>
+        <v>0.8251526166123739</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9997594748528723</v>
+        <v>0.998619872706647</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9994470809151198</v>
+        <v>0.9997295822864399</v>
       </c>
       <c r="G9" t="n">
-        <v>0.999716618812855</v>
+        <v>0.9994281803211635</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0003829850314402303</v>
+        <v>0.0002269067871810778</v>
       </c>
       <c r="I9" t="n">
-        <v>0.2097331308513057</v>
+        <v>0.2481704796469531</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0002135976611630328</v>
+        <v>0.001071937113867268</v>
       </c>
       <c r="K9" t="n">
-        <v>0.00054577089290721</v>
+        <v>0.0003462328261450901</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0003796832092399649</v>
+        <v>0.0007090837045737711</v>
       </c>
       <c r="M9" t="n">
-        <v>0.07485130550430483</v>
+        <v>0.01329219712554298</v>
       </c>
       <c r="N9" t="n">
-        <v>0.01957000335820692</v>
+        <v>0.01506342547965362</v>
       </c>
       <c r="O9" t="n">
-        <v>1.000016647631654</v>
+        <v>1.00000662657598</v>
       </c>
       <c r="P9" t="n">
-        <v>0.02040313891665751</v>
+        <v>0.01570470668791192</v>
       </c>
       <c r="Q9" t="n">
-        <v>841.7350293038977</v>
+        <v>1222.781942507945</v>
       </c>
       <c r="R9" t="n">
-        <v>1345.130744974465</v>
+        <v>1957.76406490347</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>model_22_9_2</t>
+          <t>model_22_9_10</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.9997003133011322</v>
+        <v>0.9998401316576185</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8518225699403054</v>
+        <v>0.825152644491034</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9998510721748858</v>
+        <v>0.9986198482710885</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9994853815840958</v>
+        <v>0.9997295858382638</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9997610821655097</v>
+        <v>0.9994281704741145</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0004253617661349764</v>
+        <v>0.0002269099053156607</v>
       </c>
       <c r="I10" t="n">
-        <v>0.2103163523427924</v>
+        <v>0.248170440077242</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0001322549243036063</v>
+        <v>0.001071956092828156</v>
       </c>
       <c r="K10" t="n">
-        <v>0.000507965378723279</v>
+        <v>0.0003462282785214643</v>
       </c>
       <c r="L10" t="n">
-        <v>0.000320109782367069</v>
+        <v>0.0007090959153847418</v>
       </c>
       <c r="M10" t="n">
-        <v>0.08281026590129487</v>
+        <v>0.01329213122836248</v>
       </c>
       <c r="N10" t="n">
-        <v>0.02062430037928503</v>
+        <v>0.01506352897948089</v>
       </c>
       <c r="O10" t="n">
-        <v>1.000018489667796</v>
+        <v>1.000006626667042</v>
       </c>
       <c r="P10" t="n">
-        <v>0.02150231954461861</v>
+        <v>0.01570481459394112</v>
       </c>
       <c r="Q10" t="n">
-        <v>841.5251410733644</v>
+        <v>1222.781915024296</v>
       </c>
       <c r="R10" t="n">
-        <v>1344.920856743931</v>
+        <v>1957.764037419822</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>model_22_9_1</t>
+          <t>model_22_9_9</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.9996581146346163</v>
+        <v>0.999840131240973</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8513566288921136</v>
+        <v>0.8251526354824023</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9999264110144183</v>
+        <v>0.9986198394864028</v>
       </c>
       <c r="F11" t="n">
-        <v>0.999518804212096</v>
+        <v>0.9997295873451301</v>
       </c>
       <c r="G11" t="n">
-        <v>0.9997983609110106</v>
+        <v>0.9994281709715552</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0004852566476413526</v>
+        <v>0.0002269104966834709</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2109776880240968</v>
+        <v>0.2481704528636872</v>
       </c>
       <c r="J11" t="n">
-        <v>6.53504857821053e-05</v>
+        <v>0.001071962915844286</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0004749748417246839</v>
+        <v>0.0003462263491856495</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0002701625227384563</v>
+        <v>0.0007090952985345225</v>
       </c>
       <c r="M11" t="n">
-        <v>0.09164219752813101</v>
+        <v>0.01329118128069884</v>
       </c>
       <c r="N11" t="n">
-        <v>0.02202854165943249</v>
+        <v>0.01506354860859389</v>
       </c>
       <c r="O11" t="n">
-        <v>1.000021093184497</v>
+        <v>1.000006626684312</v>
       </c>
       <c r="P11" t="n">
-        <v>0.02296634228324213</v>
+        <v>0.01570483505870609</v>
       </c>
       <c r="Q11" t="n">
-        <v>841.2616652731871</v>
+        <v>1222.781909811946</v>
       </c>
       <c r="R11" t="n">
-        <v>1344.657380943754</v>
+        <v>1957.764032207471</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>model_22_8_8</t>
+          <t>model_22_9_11</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.9995843894839793</v>
+        <v>0.9998401308786784</v>
       </c>
       <c r="D12" t="n">
-        <v>0.852032394616165</v>
+        <v>0.8251526612302235</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9994335559774675</v>
+        <v>0.9986198485121206</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9991486303415698</v>
+        <v>0.9997295813356262</v>
       </c>
       <c r="G12" t="n">
-        <v>0.9994128404597629</v>
+        <v>0.9994281696752351</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0005898987969325631</v>
+        <v>0.0002269110109080749</v>
       </c>
       <c r="I12" t="n">
-        <v>0.2100185366738304</v>
+        <v>0.2481704163183925</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0004792917946444691</v>
+        <v>0.001071955905619921</v>
       </c>
       <c r="K12" t="n">
-        <v>0.001412803526094982</v>
+        <v>0.0003462340435318827</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0009460461875388231</v>
+        <v>0.0007090969060334156</v>
       </c>
       <c r="M12" t="n">
-        <v>0.100915650340609</v>
+        <v>0.01329284944880903</v>
       </c>
       <c r="N12" t="n">
-        <v>0.02428783228146479</v>
+        <v>0.01506356567709236</v>
       </c>
       <c r="O12" t="n">
-        <v>1.000025641779909</v>
+        <v>1.000006626699329</v>
       </c>
       <c r="P12" t="n">
-        <v>0.02532181558443068</v>
+        <v>0.01570485285384587</v>
       </c>
       <c r="Q12" t="n">
-        <v>840.8711191328007</v>
+        <v>1222.78190527955</v>
       </c>
       <c r="R12" t="n">
-        <v>1344.266834803368</v>
+        <v>1957.764027675075</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>model_22_8_7</t>
+          <t>model_22_9_8</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.9995640682612773</v>
+        <v>0.9998401306675504</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8522491716422277</v>
+        <v>0.8251526255507209</v>
       </c>
       <c r="E13" t="n">
-        <v>0.999515061217402</v>
+        <v>0.9986198320415424</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9992519596158036</v>
+        <v>0.9997295868485928</v>
       </c>
       <c r="G13" t="n">
-        <v>0.9994874520825924</v>
+        <v>0.9994281689207914</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0006187418227031528</v>
+        <v>0.0002269113105735963</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2097108531529671</v>
+        <v>0.2481704669602672</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0004103268287040503</v>
+        <v>0.001071968698225519</v>
       </c>
       <c r="K13" t="n">
-        <v>0.001241333986934359</v>
+        <v>0.0003462269849335091</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0008258300682616479</v>
+        <v>0.0007090978415795138</v>
       </c>
       <c r="M13" t="n">
-        <v>0.09925943385141503</v>
+        <v>0.01329090457494794</v>
       </c>
       <c r="N13" t="n">
-        <v>0.02487452155727126</v>
+        <v>0.01506357562378854</v>
       </c>
       <c r="O13" t="n">
-        <v>1.000026895531438</v>
+        <v>1.000006626708081</v>
       </c>
       <c r="P13" t="n">
-        <v>0.02593348143732246</v>
+        <v>0.01570486322399351</v>
       </c>
       <c r="Q13" t="n">
-        <v>840.775644920004</v>
+        <v>1222.781902638292</v>
       </c>
       <c r="R13" t="n">
-        <v>1344.171360590571</v>
+        <v>1957.764025033817</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>model_22_8_6</t>
+          <t>model_22_9_12</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.999533413254032</v>
+        <v>0.9998401293909597</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8524816996959228</v>
+        <v>0.8251526697461966</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9995971553440928</v>
+        <v>0.9986198283043503</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9993591605030978</v>
+        <v>0.9997295823494765</v>
       </c>
       <c r="G14" t="n">
-        <v>0.999564213459769</v>
+        <v>0.9994281643535289</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0006622521555674636</v>
+        <v>0.0002269131225087831</v>
       </c>
       <c r="I14" t="n">
-        <v>0.2093808133348193</v>
+        <v>0.2481704042312048</v>
       </c>
       <c r="J14" t="n">
-        <v>0.000340863581240508</v>
+        <v>0.001071971600881571</v>
       </c>
       <c r="K14" t="n">
-        <v>0.001063439707909864</v>
+        <v>0.0003462327454354274</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0007021502108265363</v>
+        <v>0.0007091035052031596</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0973947800824512</v>
+        <v>0.01329256568902359</v>
       </c>
       <c r="N14" t="n">
-        <v>0.02573426034622841</v>
+        <v>0.01506363576659975</v>
       </c>
       <c r="O14" t="n">
-        <v>1.000028786842939</v>
+        <v>1.000006626760996</v>
       </c>
       <c r="P14" t="n">
-        <v>0.02682982108643015</v>
+        <v>0.0157049259272087</v>
       </c>
       <c r="Q14" t="n">
-        <v>840.6397283498047</v>
+        <v>1222.781886667929</v>
       </c>
       <c r="R14" t="n">
-        <v>1344.035444020372</v>
+        <v>1957.764009063454</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>119</v>
+        <v>19</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>model_22_8_5</t>
+          <t>model_22_9_21</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.9994894063003672</v>
+        <v>0.9998401271269179</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8527297387658093</v>
+        <v>0.8251526871187265</v>
       </c>
       <c r="E15" t="n">
-        <v>0.999678294447975</v>
+        <v>0.9986197999074812</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9994688150064071</v>
+        <v>0.9997295818070083</v>
       </c>
       <c r="G15" t="n">
-        <v>0.9996419858675643</v>
+        <v>0.9994281562545845</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0007247136381885009</v>
+        <v>0.0002269163359874211</v>
       </c>
       <c r="I15" t="n">
-        <v>0.2090287578807869</v>
+        <v>0.2481703795734206</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0002722084182084318</v>
+        <v>0.001071993656570265</v>
       </c>
       <c r="K15" t="n">
-        <v>0.0008814737811311441</v>
+        <v>0.0003462334399916723</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0005768413554841829</v>
+        <v>0.0007091135482809685</v>
       </c>
       <c r="M15" t="n">
-        <v>0.09529133640856662</v>
+        <v>0.01329013054958035</v>
       </c>
       <c r="N15" t="n">
-        <v>0.02692050590513672</v>
+        <v>0.01506374242966937</v>
       </c>
       <c r="O15" t="n">
-        <v>1.000031501924913</v>
+        <v>1.000006626854843</v>
       </c>
       <c r="P15" t="n">
-        <v>0.02806656757464802</v>
+        <v>0.01570503713114602</v>
       </c>
       <c r="Q15" t="n">
-        <v>840.4594679258888</v>
+        <v>1222.781858344703</v>
       </c>
       <c r="R15" t="n">
-        <v>1343.855183596456</v>
+        <v>1957.763980740228</v>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>model_22_8_4</t>
+          <t>model_22_9_15</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.9994282501016635</v>
+        <v>0.9998401271269179</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8529926710287036</v>
+        <v>0.8251526871187265</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9997563853610871</v>
+        <v>0.9986197999074812</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9995788232000742</v>
+        <v>0.9997295818070083</v>
       </c>
       <c r="G16" t="n">
-        <v>0.9997191404767727</v>
+        <v>0.9994281562545845</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0008115159847357041</v>
+        <v>0.0002269163359874211</v>
       </c>
       <c r="I16" t="n">
-        <v>0.208655563701195</v>
+        <v>0.2481703795734206</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0002061324558853572</v>
+        <v>0.001071993656570265</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0006989209236581259</v>
+        <v>0.0003462334399916723</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0004525279127302175</v>
+        <v>0.0007091135482809685</v>
       </c>
       <c r="M16" t="n">
-        <v>0.09291977454238948</v>
+        <v>0.01329013054958035</v>
       </c>
       <c r="N16" t="n">
-        <v>0.02848711962862697</v>
+        <v>0.01506374242966937</v>
       </c>
       <c r="O16" t="n">
-        <v>1.000035275057995</v>
+        <v>1.000006626854843</v>
       </c>
       <c r="P16" t="n">
-        <v>0.02969987528768473</v>
+        <v>0.01570503713114602</v>
       </c>
       <c r="Q16" t="n">
-        <v>840.2332129468787</v>
+        <v>1222.781858344703</v>
       </c>
       <c r="R16" t="n">
-        <v>1343.628928617446</v>
+        <v>1957.763980740228</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>121</v>
+        <v>21</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>model_22_8_3</t>
+          <t>model_22_9_14</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.9993451813284396</v>
+        <v>0.9998401271269179</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8532691489467472</v>
+        <v>0.8251526871187265</v>
       </c>
       <c r="E17" t="n">
-        <v>0.999828927768586</v>
+        <v>0.9986197999074812</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9996862502127274</v>
+        <v>0.9997295818070083</v>
       </c>
       <c r="G17" t="n">
-        <v>0.9997935104575035</v>
+        <v>0.9994281562545845</v>
       </c>
       <c r="H17" t="n">
-        <v>0.000929420049956599</v>
+        <v>0.0002269163359874211</v>
       </c>
       <c r="I17" t="n">
-        <v>0.2082631434304234</v>
+        <v>0.2481703795734206</v>
       </c>
       <c r="J17" t="n">
-        <v>0.0001447513144222854</v>
+        <v>0.001071993656570265</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0005206514013989497</v>
+        <v>0.0003462334399916723</v>
       </c>
       <c r="L17" t="n">
-        <v>0.000332701133267021</v>
+        <v>0.0007091135482809685</v>
       </c>
       <c r="M17" t="n">
-        <v>0.09024376705575979</v>
+        <v>0.01329013054958035</v>
       </c>
       <c r="N17" t="n">
-        <v>0.03048639122553863</v>
+        <v>0.01506374242966937</v>
       </c>
       <c r="O17" t="n">
-        <v>1.000040400123695</v>
+        <v>1.000006626854843</v>
       </c>
       <c r="P17" t="n">
-        <v>0.03178426001553967</v>
+        <v>0.01570503713114602</v>
       </c>
       <c r="Q17" t="n">
-        <v>839.9618995370698</v>
+        <v>1222.781858344703</v>
       </c>
       <c r="R17" t="n">
-        <v>1343.357615207637</v>
+        <v>1957.763980740228</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>Hidden Size=[20, 16], regularizer=0.2, learning_rate=0.1</t>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>model_22_9_17</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.9998401271269179</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.8251526871187265</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.9986197999074812</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.9997295818070083</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.9994281562545845</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.0002269163359874211</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.2481703795734206</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.001071993656570265</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.0003462334399916723</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.0007091135482809685</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.01329013054958035</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.01506374242966937</v>
+      </c>
+      <c r="O18" t="n">
+        <v>1.000006626854843</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.01570503713114602</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>1222.781858344703</v>
+      </c>
+      <c r="R18" t="n">
+        <v>1957.763980740228</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>model_22_9_18</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.9998401271269179</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.8251526871187265</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.9986197999074812</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.9997295818070083</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.9994281562545845</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.0002269163359874211</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.2481703795734206</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.001071993656570265</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.0003462334399916723</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.0007091135482809685</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.01329013054958035</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.01506374242966937</v>
+      </c>
+      <c r="O19" t="n">
+        <v>1.000006626854843</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.01570503713114602</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>1222.781858344703</v>
+      </c>
+      <c r="R19" t="n">
+        <v>1957.763980740228</v>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>model_22_9_19</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9998401271269179</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.8251526871187265</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.9986197999074812</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.9997295818070083</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.9994281562545845</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.0002269163359874211</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.2481703795734206</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.001071993656570265</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.0003462334399916723</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.0007091135482809685</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.01329013054958035</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.01506374242966937</v>
+      </c>
+      <c r="O20" t="n">
+        <v>1.000006626854843</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.01570503713114602</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>1222.781858344703</v>
+      </c>
+      <c r="R20" t="n">
+        <v>1957.763980740228</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>model_22_9_20</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.9998401271269179</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.8251526871187265</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.9986197999074812</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.9997295818070083</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.9994281562545845</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.0002269163359874211</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.2481703795734206</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.001071993656570265</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.0003462334399916723</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.0007091135482809685</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.01329013054958035</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.01506374242966937</v>
+      </c>
+      <c r="O21" t="n">
+        <v>1.000006626854843</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.01570503713114602</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>1222.781858344703</v>
+      </c>
+      <c r="R21" t="n">
+        <v>1957.763980740228</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>model_22_9_16</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0.9998401271269179</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.8251526871187265</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.9986197999074812</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.9997295818070083</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.9994281562545845</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.0002269163359874211</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.2481703795734206</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.001071993656570265</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.0003462334399916723</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.0007091135482809685</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.01329013054958035</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.01506374242966937</v>
+      </c>
+      <c r="O22" t="n">
+        <v>1.000006626854843</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.01570503713114602</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>1222.781858344703</v>
+      </c>
+      <c r="R22" t="n">
+        <v>1957.763980740228</v>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>model_22_9_22</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0.9998401271269179</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.8251526871187265</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.9986197999074812</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.9997295818070083</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.9994281562545845</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.0002269163359874211</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.2481703795734206</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.001071993656570265</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.0003462334399916723</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.0007091135482809685</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.01329013054958035</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.01506374242966937</v>
+      </c>
+      <c r="O23" t="n">
+        <v>1.000006626854843</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0.01570503713114602</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>1222.781858344703</v>
+      </c>
+      <c r="R23" t="n">
+        <v>1957.763980740228</v>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>model_22_9_24</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0.9998401271269179</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.8251526871187265</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.9986197999074812</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.9997295818070083</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.9994281562545845</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.0002269163359874211</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.2481703795734206</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.001071993656570265</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.0003462334399916723</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.0007091135482809685</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.01329013054958035</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.01506374242966937</v>
+      </c>
+      <c r="O24" t="n">
+        <v>1.000006626854843</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.01570503713114602</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>1222.781858344703</v>
+      </c>
+      <c r="R24" t="n">
+        <v>1957.763980740228</v>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>model_22_9_23</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0.9998401271269179</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.8251526871187265</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.9986197999074812</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.9997295818070083</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.9994281562545845</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.0002269163359874211</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.2481703795734206</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.001071993656570265</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.0003462334399916723</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.0007091135482809685</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.01329013054958035</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.01506374242966937</v>
+      </c>
+      <c r="O25" t="n">
+        <v>1.000006626854843</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0.01570503713114602</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>1222.781858344703</v>
+      </c>
+      <c r="R25" t="n">
+        <v>1957.763980740228</v>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>model_22_9_13</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0.9998401271269179</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.8251526871187265</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.9986197999074812</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.9997295818070083</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.9994281562545845</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.0002269163359874211</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.2481703795734206</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.001071993656570265</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.0003462334399916723</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.0007091135482809685</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.01329013054958035</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.01506374242966937</v>
+      </c>
+      <c r="O26" t="n">
+        <v>1.000006626854843</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.01570503713114602</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>1222.781858344703</v>
+      </c>
+      <c r="R26" t="n">
+        <v>1957.763980740228</v>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>Hidden Size=[30, 16], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>model_14_9_7</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0.9981124142656811</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.7726438602367558</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.9977683809693192</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.9989800096949198</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.9989787890124103</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.002679153945484949</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.3226990370833143</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.003612276000999758</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.001644732542305455</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.002628504307573246</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.3232964687122324</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.05176054429278105</v>
+      </c>
+      <c r="O27" t="n">
+        <v>1.000296091879893</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.05396409782242253</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>365.8445084525676</v>
+      </c>
+      <c r="R27" t="n">
+        <v>581.5855294542391</v>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>Hidden Size=[12, 10], regularizer=0.2, learning_rate=0.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>model_14_9_6</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0.9979014074876565</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.7721983594772649</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.9981184626205238</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.9991418179388237</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.9991395524689388</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.00297864743687463</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.3233313607419466</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.003045606005068</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.001383817038465307</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.002214713775429761</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.3062728783231869</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.05457698633008817</v>
+      </c>
+      <c r="O28" t="n">
+        <v>1.000329190982328</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.05690044162809656</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>365.6325719234861</v>
+      </c>
+      <c r="R28" t="n">
+        <v>581.3735929251576</v>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>Hidden Size=[12, 10], regularizer=0.2, learning_rate=0.1</t>
         </is>
       </c>
     </row>

</xml_diff>